<commit_message>
Added annual exam paper part 2
</commit_message>
<xml_diff>
--- a/Question paper/Annual Examination/New Exam Routine.xlsx
+++ b/Question paper/Annual Examination/New Exam Routine.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mydisk_school\Question paper\Annual Examination\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A7145F-653E-4F23-88A1-57142C72DDF7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DEEA26A-E256-4548-B94D-70873D3ABA5E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -573,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -583,9 +583,9 @@
     <col min="2" max="2" width="16" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.109375" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.44140625" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="8.88671875" style="5"/>
   </cols>
@@ -779,13 +779,13 @@
       <c r="B9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F9" s="6" t="s">
@@ -811,7 +811,7 @@
       <c r="E10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="6" t="s">
         <v>19</v>
       </c>
       <c r="G10" s="4"/>
@@ -822,7 +822,7 @@
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="6" t="s">
@@ -848,7 +848,7 @@
       <c r="B12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D12" s="6" t="s">
@@ -863,7 +863,7 @@
       <c r="G12" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="6" t="s">
         <v>21</v>
       </c>
       <c r="I12" s="6" t="s">

</xml_diff>

<commit_message>
Added final exam paper part 3
</commit_message>
<xml_diff>
--- a/Question paper/Annual Examination/New Exam Routine.xlsx
+++ b/Question paper/Annual Examination/New Exam Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mydisk_school\Question paper\Annual Examination\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DEEA26A-E256-4548-B94D-70873D3ABA5E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F97D8B6-3EBD-4B8E-A748-63AEE103490A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,7 +574,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -707,16 +707,16 @@
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="B6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="6" t="s">
         <v>15</v>
       </c>
       <c r="F6" s="6" t="s">
@@ -736,10 +736,10 @@
       <c r="C7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F7" s="6" t="s">
@@ -762,10 +762,10 @@
       <c r="D8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="6" t="s">
         <v>13</v>
       </c>
       <c r="G8" s="4"/>

</xml_diff>

<commit_message>
Added all paper except 3,4 nepali and 8 science, computer
</commit_message>
<xml_diff>
--- a/Question paper/Annual Examination/New Exam Routine.xlsx
+++ b/Question paper/Annual Examination/New Exam Routine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mydisk_school\Question paper\Annual Examination\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F97D8B6-3EBD-4B8E-A748-63AEE103490A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E8CEE2-9AB0-40B1-B7F1-9D8502BF55A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -255,7 +255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -263,7 +263,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -306,6 +305,77 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>16234</xdr:colOff>
+          <xdr:row>25</xdr:row>
+          <xdr:rowOff>205077</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>9</xdr:col>
+          <xdr:colOff>23854</xdr:colOff>
+          <xdr:row>38</xdr:row>
+          <xdr:rowOff>205078</xdr:rowOff>
+        </xdr:to>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="2" name="Picture 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0078ABAA-1668-4C77-AF50-161FC8AE37E8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+              <a:extLst>
+                <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
+                  <a14:cameraTool cellRange="$A$1:$I$13" spid="_x0000_s1077"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+            <a:srcRect/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="16234" y="5989651"/>
+              <a:ext cx="9595568" cy="3014870"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -570,23 +640,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="12.109375" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.5546875" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
@@ -623,85 +693,85 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="8" t="s">
+      <c r="B2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="10"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="9"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="7" t="s">
+      <c r="B3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="13"/>
+      <c r="E3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="10"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="12"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="13"/>
+      <c r="C4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="10"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="12"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="7" t="s">
+      <c r="B5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="16"/>
+      <c r="D5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="13"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="15"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
@@ -713,7 +783,7 @@
       <c r="C6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E6" s="6" t="s">
@@ -730,7 +800,7 @@
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -756,7 +826,7 @@
       <c r="B8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D8" s="4" t="s">
@@ -776,7 +846,7 @@
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="6" t="s">
@@ -802,13 +872,13 @@
       <c r="B10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="6" t="s">
         <v>14</v>
       </c>
       <c r="F10" s="6" t="s">
@@ -880,7 +950,7 @@
       <c r="C13" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E13" s="6" t="s">
@@ -905,5 +975,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added admission ads and partial result
</commit_message>
<xml_diff>
--- a/Question paper/Annual Examination/New Exam Routine.xlsx
+++ b/Question paper/Annual Examination/New Exam Routine.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mydisk_school\Question paper\Annual Examination\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E49A0E1-6244-47C2-8C61-6C240062D874}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F166C00-3F93-4819-8997-E06E0AFE0F73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
+    <sheet name="Routine" sheetId="1" r:id="rId1"/>
+    <sheet name="Information" sheetId="2" r:id="rId2"/>
+    <sheet name="Ledger" sheetId="3" r:id="rId3"/>
+    <sheet name="absents" sheetId="4" r:id="rId4"/>
+    <sheet name="viber status" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,8 +28,814 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>imksav</author>
+  </authors>
+  <commentList>
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{F5D47ED2-0AD3-469A-A652-D8C6E2D0DE91}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>imksav:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Many absents but in all subjects they are amisha, david, milvin, som, sonam, sumisha</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{E2285CA3-F4F4-4173-82AC-0523FC7710A9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>imksav:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Yur absent on all subjects</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{358B7251-7A42-46D4-8687-5BB32AD6A9E9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>imksav:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Jonex absent on nepali only and jeevan in all</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{24CBD73B-6886-4624-9430-F5725D037632}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>imksav:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Samyog Baniya absent in English
+in all subjects: deepa, krijol, krish, mamata, pawan, prasahana</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E6" authorId="0" shapeId="0" xr:uid="{D100A399-208B-4556-B33C-370D85753764}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>imksav:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+absent students: deepa, krijol, krish, mamta, pawan, samyog</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{2B91402F-B979-49DD-8D5D-E3359AFBD499}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>imksav:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+asim, mithun, sadikshya, simran, sushant</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{36F46F7C-96B6-4803-885D-1531E675A953}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>imksav:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+asim, sadikshya, simran, sushant</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F7" authorId="0" shapeId="0" xr:uid="{A9A8A765-DF9D-436D-A2C5-CC399A183464}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>imksav:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+absent students: sadikshya, simran, sushant</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C8" authorId="0" shapeId="0" xr:uid="{7D3C2D1C-45A7-4DD0-AE61-E3802BE32AFD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>imksav:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+absent student: atit</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{0A4B06A4-C325-460B-88A0-36CC8F65EDC4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>imksav:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+absent student: atit</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{3618AED2-67F3-452C-A846-2C7F8D35D5AB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>imksav:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+absent: atit baral
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F8" authorId="0" shapeId="0" xr:uid="{5478F076-52A5-46AC-BFDB-FD572871F893}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>imksav:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+absent students: atit, sujata</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{DBBDC056-AA05-4456-89A0-DD5640EA68C7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>imksav:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+absent students:
+alisha, basanta, biwesh, jyoti, samir, sampana, shiva, siddhartha, sudip</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{EDC4FD58-6651-4501-89D3-0C1042F9A316}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>imksav:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+absent students:
+alisha, biwesh, jyoti, samir, sampana, shiva, siddhartha</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{660E85EA-7F7D-4971-96D8-BE288B751C08}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>imksav:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+absent: biwesh, jyoti, samir, sampana, shiva, siddhartha</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{5E6730A5-7D15-4AC7-B2A7-4494C03562EE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>imksav:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+absent students: bimala, sagar, prizma, sonam</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D10" authorId="0" shapeId="0" xr:uid="{2B7D6086-3253-490D-9077-D402DFD09279}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>imksav:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+absent: anjela, ashish, bimala, prizma, purnima, sagar, sonam, sumina, yujina</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{B3F2EC33-6EBC-4F48-B815-43FCD561F51A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>imksav:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+absent: ashish, bimala, prizma, sagar, sonam</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{D4B1355A-A40E-4A42-AABD-B611D410A412}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>imksav:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+absent student: prizma kharel, bimala, sagar</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{73D639CA-33E1-4A64-BF1F-F7D8B6C331B0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>imksav:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+absent: bijan kafle</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{A71E6662-5A26-480B-B90A-1526AADBE6F6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>imksav:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+absent: bijan kafle</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D11" authorId="0" shapeId="0" xr:uid="{BCE5A05E-95ED-4A4E-AFEF-86A6962B7F22}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>imksav:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+absent student: bijan</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F11" authorId="0" shapeId="0" xr:uid="{B88C7F14-CE85-43D1-A1D9-BB04CED55568}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>imksav:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+absent: bijan kafle</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{115276B3-2A19-49D5-9987-75AC19F83954}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>imksav:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+absent: babita, dawa</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{8689A0C1-A94F-4B5D-8F0C-8EE5AB957F4F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>imksav:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+absent: babita, dawa</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{46FE6D1D-19B1-49B9-9504-8F62DA880C17}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>imksav:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+absent students: dawa, babita</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H12" authorId="0" shapeId="0" xr:uid="{D043241A-D234-4462-907B-C84EF9DB99D9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>imksav:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+absent students: dawa, babita</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{5393D9A6-29A1-4397-A041-695C16D427C4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>imksav:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+absent: karan, roman, sumina</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D13" authorId="0" shapeId="0" xr:uid="{433969A4-A982-4F90-A674-F49072335D91}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>imksav:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+absent: karan, roman</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F13" authorId="0" shapeId="0" xr:uid="{8624132A-2C71-4EBC-895F-E06C02C8273B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>imksav:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+absent student: karan</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G13" authorId="0" shapeId="0" xr:uid="{842C5EA6-A497-4C89-A12F-7F6122459B84}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>imksav:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+absent students: karan, roman</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H13" authorId="0" shapeId="0" xr:uid="{CCCA5354-474D-4825-AFE3-50A85ED3B265}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>imksav:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+absent student: karan</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I13" authorId="0" shapeId="0" xr:uid="{838272C0-4FBE-4D1B-9EF9-262E33D57CCB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>imksav:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+absent students: karan, roman</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="361">
   <si>
     <t>Nurs</t>
   </si>
@@ -206,13 +1015,981 @@
   </si>
   <si>
     <t>All the teachers will provide the link 15 minutes before your exam starts.</t>
+  </si>
+  <si>
+    <t>Moral Education</t>
+  </si>
+  <si>
+    <t>shanti,yamuna</t>
+  </si>
+  <si>
+    <t>shanti</t>
+  </si>
+  <si>
+    <t>Nursery</t>
+  </si>
+  <si>
+    <t>Class VIII</t>
+  </si>
+  <si>
+    <t>Class VII</t>
+  </si>
+  <si>
+    <t>Class VI</t>
+  </si>
+  <si>
+    <t>ALISHA YASMALI MAGAR</t>
+  </si>
+  <si>
+    <t>ALON SHRESTHA</t>
+  </si>
+  <si>
+    <t>AMAN KUMAR YADAV</t>
+  </si>
+  <si>
+    <t>ANGKAJI SHERPA</t>
+  </si>
+  <si>
+    <t>ANSUMA TAMANG</t>
+  </si>
+  <si>
+    <t>ANUSH TAMANG</t>
+  </si>
+  <si>
+    <t>APSAN THAPA</t>
+  </si>
+  <si>
+    <t>ARISHMA GHIMIRE</t>
+  </si>
+  <si>
+    <t>BABITA GHIMIRE</t>
+  </si>
+  <si>
+    <t>DAWA LHAMO GURUNG</t>
+  </si>
+  <si>
+    <t>DIPIKA SIGDEL</t>
+  </si>
+  <si>
+    <t>GARIMA ROSHYARA</t>
+  </si>
+  <si>
+    <t>ISHAN CHAND</t>
+  </si>
+  <si>
+    <t>KRISHNA GURUNG</t>
+  </si>
+  <si>
+    <t>KRISHU GURUNG</t>
+  </si>
+  <si>
+    <t>LIZA RAI</t>
+  </si>
+  <si>
+    <t>MANISHA YADAV</t>
+  </si>
+  <si>
+    <t>MANJIT ADHIKARI</t>
+  </si>
+  <si>
+    <t>NULAN MAGAR</t>
+  </si>
+  <si>
+    <t>PRAMILA KARKI</t>
+  </si>
+  <si>
+    <t>PRIJANA NEUPANE</t>
+  </si>
+  <si>
+    <t>PRIYA KUMARI MAHATO</t>
+  </si>
+  <si>
+    <t>PUSHPA KUMARI MAHATO</t>
+  </si>
+  <si>
+    <t>RAJESH RAY</t>
+  </si>
+  <si>
+    <t>ROSHIKA GHISING</t>
+  </si>
+  <si>
+    <t>RUSSELL BUDHA MAGAR</t>
+  </si>
+  <si>
+    <t>SAMIR DULAL</t>
+  </si>
+  <si>
+    <t>SAMITA KC</t>
+  </si>
+  <si>
+    <t>SANMI TAMANG</t>
+  </si>
+  <si>
+    <t>SARBIN POUDEL</t>
+  </si>
+  <si>
+    <t>SAUGAT THAPA MAGAR</t>
+  </si>
+  <si>
+    <t>SAURYA POUDEL</t>
+  </si>
+  <si>
+    <t>SUBASHNA PAKHRIN</t>
+  </si>
+  <si>
+    <t>SUMIT KARKI</t>
+  </si>
+  <si>
+    <t>SWIKRITI KARKI</t>
+  </si>
+  <si>
+    <t>UDAYKANT THAKUR</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>AASHIM GURUNG</t>
+  </si>
+  <si>
+    <t>AMISHA SHARMA</t>
+  </si>
+  <si>
+    <t>DAIMOND GURUNG</t>
+  </si>
+  <si>
+    <t>DEEYA ROKKA</t>
+  </si>
+  <si>
+    <t>GAUTAM GURUNG</t>
+  </si>
+  <si>
+    <t>JEEBRAJ MAHATARA</t>
+  </si>
+  <si>
+    <t>JONISHA GHIMIRE</t>
+  </si>
+  <si>
+    <t>KABIR MAHARJAN</t>
+  </si>
+  <si>
+    <t>KARAN POUDELI</t>
+  </si>
+  <si>
+    <t>LABAHANG SAUDEN</t>
+  </si>
+  <si>
+    <t>MOLIKA SHRESTHA</t>
+  </si>
+  <si>
+    <t>PAYAL TAMANG</t>
+  </si>
+  <si>
+    <t>POOJNESS KUMAR MAHATO</t>
+  </si>
+  <si>
+    <t>PRANIDHI RANA</t>
+  </si>
+  <si>
+    <t>REBA ACHARYA</t>
+  </si>
+  <si>
+    <t>ROMAN RANA MAGAR</t>
+  </si>
+  <si>
+    <t>ROSHAN SINGH DHAMI</t>
+  </si>
+  <si>
+    <t>SAMMAN JOSHI</t>
+  </si>
+  <si>
+    <t>SANJEEB GIRI</t>
+  </si>
+  <si>
+    <t>SARITA DHAMI</t>
+  </si>
+  <si>
+    <t>SIJAN THAPA MAGAR</t>
+  </si>
+  <si>
+    <t>SUHAJA KARKI</t>
+  </si>
+  <si>
+    <t>SUMNIMA SHERPA</t>
+  </si>
+  <si>
+    <t>UNIQUE ADHIKARI</t>
+  </si>
+  <si>
+    <t>YANGCHEN SHERPA</t>
+  </si>
+  <si>
+    <t>Class IX</t>
+  </si>
+  <si>
+    <t>AASHRIYA NEPAL</t>
+  </si>
+  <si>
+    <t>ABIKAL MUKHIYA</t>
+  </si>
+  <si>
+    <t>ANSHAL SHAH</t>
+  </si>
+  <si>
+    <t>ARJUN MAHATARA</t>
+  </si>
+  <si>
+    <t>ASHMITA KHATRI</t>
+  </si>
+  <si>
+    <t>ASIM TANDAN</t>
+  </si>
+  <si>
+    <t>BIBEK NARAYAN SHREST</t>
+  </si>
+  <si>
+    <t>BINISHA BHANDARI</t>
+  </si>
+  <si>
+    <t>BINU TAMANG</t>
+  </si>
+  <si>
+    <t>BISHWAS UPADHYAYA</t>
+  </si>
+  <si>
+    <t>DEEPAK PAHARI</t>
+  </si>
+  <si>
+    <t>DIPAK JIREL</t>
+  </si>
+  <si>
+    <t>DOLMA SHERPA</t>
+  </si>
+  <si>
+    <t>JESICA GURUNG</t>
+  </si>
+  <si>
+    <t>KIRAN PALPALI KHADKA</t>
+  </si>
+  <si>
+    <t>KOSHISH GURUNG</t>
+  </si>
+  <si>
+    <t>KUNJANG SHERPA</t>
+  </si>
+  <si>
+    <t>LAXMAN BHATTARAI</t>
+  </si>
+  <si>
+    <t>MILA SHRESTHA</t>
+  </si>
+  <si>
+    <t>MITRABANDHU SIGDEL</t>
+  </si>
+  <si>
+    <t>PRAJESH THAPALIYA</t>
+  </si>
+  <si>
+    <t>PRINCE BINOD ARYAL</t>
+  </si>
+  <si>
+    <t>RENU TAMANG</t>
+  </si>
+  <si>
+    <t>RUPA SUBEDI</t>
+  </si>
+  <si>
+    <t>SABHYATA JOSHI</t>
+  </si>
+  <si>
+    <t>SAJINA MAHARJAN</t>
+  </si>
+  <si>
+    <t>SALINA BASNET</t>
+  </si>
+  <si>
+    <t>SAMI MISHRA</t>
+  </si>
+  <si>
+    <t>SAMIKSHA SHRESTHA</t>
+  </si>
+  <si>
+    <t>SAMJHANA DONG</t>
+  </si>
+  <si>
+    <t>SAMUEL SINGH LAL</t>
+  </si>
+  <si>
+    <t>SHANTIKA KC</t>
+  </si>
+  <si>
+    <t>SOHIT GHATANE</t>
+  </si>
+  <si>
+    <t>SONIM MANANDHAR</t>
+  </si>
+  <si>
+    <t>SONIR SHRESTHA</t>
+  </si>
+  <si>
+    <t>STUTI BASNET</t>
+  </si>
+  <si>
+    <t>SUBHAM SHRESTHA</t>
+  </si>
+  <si>
+    <t>SUCHAN GURUNG</t>
+  </si>
+  <si>
+    <t>SUMI TAMANG</t>
+  </si>
+  <si>
+    <t>SUPRIYA SHRESTHA</t>
+  </si>
+  <si>
+    <t>UGESH KATWAL</t>
+  </si>
+  <si>
+    <t>AARYA KHADKA</t>
+  </si>
+  <si>
+    <t>AARYAN KC</t>
+  </si>
+  <si>
+    <t>AASIMA BANIYA</t>
+  </si>
+  <si>
+    <t>ABHISEKH SHAHI</t>
+  </si>
+  <si>
+    <t>ADRINA WAGLE</t>
+  </si>
+  <si>
+    <t>ANGEL LAMA</t>
+  </si>
+  <si>
+    <t>APSARA KHATRI</t>
+  </si>
+  <si>
+    <t>BASANTA ROKAYA</t>
+  </si>
+  <si>
+    <t>BIJAN SATYAL</t>
+  </si>
+  <si>
+    <t>BISHAL LAMA</t>
+  </si>
+  <si>
+    <t>BISHWANT KC</t>
+  </si>
+  <si>
+    <t>DEBISHA SHRESTHA</t>
+  </si>
+  <si>
+    <t>GOVINDA ROKKA</t>
+  </si>
+  <si>
+    <t>JESIN GURUNG</t>
+  </si>
+  <si>
+    <t>KAMALA KEPCHHAKI MAGAR</t>
+  </si>
+  <si>
+    <t>KRIPA TAMANG</t>
+  </si>
+  <si>
+    <t>NABIN GURUNG</t>
+  </si>
+  <si>
+    <t>NARENDRA MAHATARA</t>
+  </si>
+  <si>
+    <t>NIDHI KARKI</t>
+  </si>
+  <si>
+    <t>NILU TAMANG</t>
+  </si>
+  <si>
+    <t>OM PRAKASH THAKUR</t>
+  </si>
+  <si>
+    <t>PRANISH RAI</t>
+  </si>
+  <si>
+    <t>PRASANNATA KARKI</t>
+  </si>
+  <si>
+    <t>PRASHANTI TAMANG</t>
+  </si>
+  <si>
+    <t>PREM CHAUDHARY</t>
+  </si>
+  <si>
+    <t>PRIYANSHI POUDEL</t>
+  </si>
+  <si>
+    <t>SABUKH RAI</t>
+  </si>
+  <si>
+    <t>SANJOG BANIYA</t>
+  </si>
+  <si>
+    <t>SANSKRITI BOHARA</t>
+  </si>
+  <si>
+    <t>SAUGAT SIGDEL</t>
+  </si>
+  <si>
+    <t>SIRJNA ALE</t>
+  </si>
+  <si>
+    <t>SUMITRA TAMANG</t>
+  </si>
+  <si>
+    <t>SUVARNA LAMSAL</t>
+  </si>
+  <si>
+    <t>SWOPNIL BASNET</t>
+  </si>
+  <si>
+    <t>TRISHA REGMI</t>
+  </si>
+  <si>
+    <t>TSHERING YANJI SHERPA</t>
+  </si>
+  <si>
+    <t>UGEN FUNCHOK SHERPA</t>
+  </si>
+  <si>
+    <t>UGIN LAMA</t>
+  </si>
+  <si>
+    <t>UPAMA HAMAL</t>
+  </si>
+  <si>
+    <t>Class V</t>
+  </si>
+  <si>
+    <t>AAKASH SUBEDI</t>
+  </si>
+  <si>
+    <t>ANJELA SHRESTHA</t>
+  </si>
+  <si>
+    <t>ASHISH MAHATARA</t>
+  </si>
+  <si>
+    <t>BALA CHAUHAN</t>
+  </si>
+  <si>
+    <t>BIMALA TAMANG</t>
+  </si>
+  <si>
+    <t>DEEPSON PAHARI</t>
+  </si>
+  <si>
+    <t>HEMA SHERCHAN</t>
+  </si>
+  <si>
+    <t>KANISKA NEUPANE</t>
+  </si>
+  <si>
+    <t>LIZEN RAI</t>
+  </si>
+  <si>
+    <t>MITHILESH RAY</t>
+  </si>
+  <si>
+    <t>NITIKA THIN TAMANG</t>
+  </si>
+  <si>
+    <t>NUMA LIMBU</t>
+  </si>
+  <si>
+    <t>PEMA TAMANG</t>
+  </si>
+  <si>
+    <t>PRASHNA ADHIKARI</t>
+  </si>
+  <si>
+    <t>PRINCE NEUPANE</t>
+  </si>
+  <si>
+    <t>PRIZMA KHAREL</t>
+  </si>
+  <si>
+    <t>PURNIMA BASNET</t>
+  </si>
+  <si>
+    <t>SAFIYA KHADKA</t>
+  </si>
+  <si>
+    <t>SAGAR THAPA</t>
+  </si>
+  <si>
+    <t>SAMRIDDHI GURUNG</t>
+  </si>
+  <si>
+    <t>SANDIP GIRI</t>
+  </si>
+  <si>
+    <t>SARISHMA SHAHI</t>
+  </si>
+  <si>
+    <t>SARITA DONG</t>
+  </si>
+  <si>
+    <t>SAROJ SINGH DHAMI</t>
+  </si>
+  <si>
+    <t>SHUBHAM LAMA</t>
+  </si>
+  <si>
+    <t>SONAM BARMA</t>
+  </si>
+  <si>
+    <t>SONISKA SHRESTHA</t>
+  </si>
+  <si>
+    <t>SUMINA  THAPA</t>
+  </si>
+  <si>
+    <t>SWIKRITI KHADKA</t>
+  </si>
+  <si>
+    <t>TASHI TENJING SHERPA</t>
+  </si>
+  <si>
+    <t>YUJINA TAMANG</t>
+  </si>
+  <si>
+    <t>YUWON SHAHI</t>
+  </si>
+  <si>
+    <t>Class IV</t>
+  </si>
+  <si>
+    <t>AAROHI PYAKUREL</t>
+  </si>
+  <si>
+    <t>ALISHA TAMANG</t>
+  </si>
+  <si>
+    <t>ANKITA YADAV</t>
+  </si>
+  <si>
+    <t>BASANTA DHAKAL</t>
+  </si>
+  <si>
+    <t>BIWESH SATYAL</t>
+  </si>
+  <si>
+    <t>DARSH THAPA</t>
+  </si>
+  <si>
+    <t>DIBIKSHYA RAI</t>
+  </si>
+  <si>
+    <t>JAMUNA TAMANG</t>
+  </si>
+  <si>
+    <t>JYOTI TAMANG</t>
+  </si>
+  <si>
+    <t>KABITA GIRI</t>
+  </si>
+  <si>
+    <t>LAMIN TAMANG</t>
+  </si>
+  <si>
+    <t>NGAWANG FING SHERPA</t>
+  </si>
+  <si>
+    <t>PARI SHRESTHA</t>
+  </si>
+  <si>
+    <t>PRAJWAL ADHIKARI</t>
+  </si>
+  <si>
+    <t>PRINCE KR MAHATO</t>
+  </si>
+  <si>
+    <t>PUJA KATWAL</t>
+  </si>
+  <si>
+    <t>RUBY RAI</t>
+  </si>
+  <si>
+    <t>SADIKSHYA POUDEL</t>
+  </si>
+  <si>
+    <t>SAMIR RAYAMAJHI</t>
+  </si>
+  <si>
+    <t>SAMJHANA TAMANG</t>
+  </si>
+  <si>
+    <t>SAMPANA SHRESTHA</t>
+  </si>
+  <si>
+    <t>SAMRIDDHI SHRESTHA</t>
+  </si>
+  <si>
+    <t>SAMRIDHI RAI</t>
+  </si>
+  <si>
+    <t>SANSHILA TAMANG</t>
+  </si>
+  <si>
+    <t>SHIVA SHRESTHA</t>
+  </si>
+  <si>
+    <t>SHREYA SHRESTHA</t>
+  </si>
+  <si>
+    <t>SIDDHARTHA THAPA</t>
+  </si>
+  <si>
+    <t>SOFY TAMANG</t>
+  </si>
+  <si>
+    <t>SUDIP GURUNG</t>
+  </si>
+  <si>
+    <t>Class III</t>
+  </si>
+  <si>
+    <t>AARAMBHA GC</t>
+  </si>
+  <si>
+    <t>AARYA ROSHYARA</t>
+  </si>
+  <si>
+    <t>AAYUSH PANDIT</t>
+  </si>
+  <si>
+    <t>ANUP THAPA</t>
+  </si>
+  <si>
+    <t>ATIT BARAL</t>
+  </si>
+  <si>
+    <t>DIBASIS KARKI</t>
+  </si>
+  <si>
+    <t>DIPESH SIGDEL</t>
+  </si>
+  <si>
+    <t>DIPSHAN GURUNG</t>
+  </si>
+  <si>
+    <t>JENIKA GURUNG</t>
+  </si>
+  <si>
+    <t>JONISH GHIMIRE</t>
+  </si>
+  <si>
+    <t>KHUSHI RIMAL</t>
+  </si>
+  <si>
+    <t>PRATIBHA KUNWAR</t>
+  </si>
+  <si>
+    <t>RIJAN BAJAGAIN</t>
+  </si>
+  <si>
+    <t>RITISHA SHRESTHA</t>
+  </si>
+  <si>
+    <t>SAURAV PULAMI MAGAR</t>
+  </si>
+  <si>
+    <t>SAURAV RAI</t>
+  </si>
+  <si>
+    <t>SESELIYA KHAYAHANG</t>
+  </si>
+  <si>
+    <t>SIMRAN DHAKAL</t>
+  </si>
+  <si>
+    <t>SUDIKSHYA SHRESTHA</t>
+  </si>
+  <si>
+    <t>SUJATA TAMANG</t>
+  </si>
+  <si>
+    <t>SUVECHCHHA THAPA</t>
+  </si>
+  <si>
+    <t>SUYOG SHRESTHA</t>
+  </si>
+  <si>
+    <t>UPSON KHATRI</t>
+  </si>
+  <si>
+    <t>Class II</t>
+  </si>
+  <si>
+    <t>ANISKA SHRESTHA</t>
+  </si>
+  <si>
+    <t>ARNAV GIRI</t>
+  </si>
+  <si>
+    <t>ASHIM PRASAI</t>
+  </si>
+  <si>
+    <t>AYUSH SUBEDI</t>
+  </si>
+  <si>
+    <t>BINAM KHADKA</t>
+  </si>
+  <si>
+    <t>JENISHA RAYA CHHETRI</t>
+  </si>
+  <si>
+    <t>KARISHMA SHRESTHA</t>
+  </si>
+  <si>
+    <t>KASHYAP PANDEY</t>
+  </si>
+  <si>
+    <t>KRISHMA RAI</t>
+  </si>
+  <si>
+    <t>KUSHAL GAUTAM</t>
+  </si>
+  <si>
+    <t>MITHUN RAYA</t>
+  </si>
+  <si>
+    <t>RUDRA ALE</t>
+  </si>
+  <si>
+    <t>SADIKSHA PAUDEL</t>
+  </si>
+  <si>
+    <t>SAUGAT RAI</t>
+  </si>
+  <si>
+    <t>SHARAS KHATRI KC</t>
+  </si>
+  <si>
+    <t>SHREETI BAJIMAYA</t>
+  </si>
+  <si>
+    <t>SIMRAN LAMA</t>
+  </si>
+  <si>
+    <t>SONIYA PAHARI</t>
+  </si>
+  <si>
+    <t>SUBODH BASNET</t>
+  </si>
+  <si>
+    <t>SUSAN KC</t>
+  </si>
+  <si>
+    <t>SUSHANT LAMA</t>
+  </si>
+  <si>
+    <t>YUG BASNET</t>
+  </si>
+  <si>
+    <t>ABDUL AJIJ MANSURI</t>
+  </si>
+  <si>
+    <t>BEEPTI SHRESTHA</t>
+  </si>
+  <si>
+    <t>BINUSHA TAMANG</t>
+  </si>
+  <si>
+    <t>DEEPA RAI</t>
+  </si>
+  <si>
+    <t>KHUSHI THAPA</t>
+  </si>
+  <si>
+    <t>KRIJOL GURUNG</t>
+  </si>
+  <si>
+    <t>KRISH ADHIKARI</t>
+  </si>
+  <si>
+    <t>KRISH PRADHAN</t>
+  </si>
+  <si>
+    <t>KRITAN SHRESTHA</t>
+  </si>
+  <si>
+    <t>MAMTA TAMANG</t>
+  </si>
+  <si>
+    <t>PAWAN TAMANG</t>
+  </si>
+  <si>
+    <t>PRASHANA POUDEL</t>
+  </si>
+  <si>
+    <t>RACHEL UPADHAYAYA</t>
+  </si>
+  <si>
+    <t>RAKHI THAKUR</t>
+  </si>
+  <si>
+    <t>RAYAN BUDHA MAGAR</t>
+  </si>
+  <si>
+    <t>SAMYOG BANIYA</t>
+  </si>
+  <si>
+    <t>SANGAM KUMAR CHAUDH</t>
+  </si>
+  <si>
+    <t>SARIKA POUDEL</t>
+  </si>
+  <si>
+    <t>SUZUKA ADHIKARI</t>
+  </si>
+  <si>
+    <t>SWIKRIT KARKI</t>
+  </si>
+  <si>
+    <t>TENISHA ROKAYA</t>
+  </si>
+  <si>
+    <t>YUPESH TAMANG</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Class I</t>
+  </si>
+  <si>
+    <t>Jonex absent on nepali only and jeevan in all</t>
+  </si>
+  <si>
+    <t>In Science, Maths, Social, English: Bijan</t>
+  </si>
+  <si>
+    <t>All are present</t>
+  </si>
+  <si>
+    <r>
+      <t>Acc./</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Comp.</t>
+    </r>
+  </si>
+  <si>
+    <t>In English: Karan, Roman, Sumina
+In Social: Karan, Roman
+In HPE: Karan
+In Computer: Karan, Roman
+In OBTE: Karan, Roman
+In Science: Karan</t>
+  </si>
+  <si>
+    <t>yamuna</t>
+  </si>
+  <si>
+    <t>sas, yamuna</t>
+  </si>
+  <si>
+    <t>kapil, dinesh</t>
+  </si>
+  <si>
+    <t>In maths, social, science: Babita, Dawa</t>
+  </si>
+  <si>
+    <t>sandeep, kapil</t>
+  </si>
+  <si>
+    <t>In all subjects: amisha, david, milvin, som, sonam, sumisha</t>
+  </si>
+  <si>
+    <t>In all subjects: yur</t>
+  </si>
+  <si>
+    <t>In Maths: asim, mithun, sadikshya, simran, sushant
+In Science: asim, sadikshya, simran, sushant
+In Nepali: sadikshya, simran, sushant
+In Social, Moral, English: Sadikshya, Simran, Sushant</t>
+  </si>
+  <si>
+    <t>In English: Samyog
+In Nepali: deepa, krijol, krish, mamta, pawan, samyog
+In math, sajilo serophero: deepa, krijol, krish, mamata, pawan</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In Social: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>ashish</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, bimala, prizma, sagar, sonam
+In English: prizma kharel, bimala, sagar
+In Maths: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>anjela, ashish, bimala, prizma, purnima, sagar, sonam, sumina, yujina</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+In Science: bimala, sagar, prizma, sonam</t>
+    </r>
+  </si>
+  <si>
+    <t>In maths,science, english, nepali: atit
+In Social and Moral: atit, sujata</t>
+  </si>
+  <si>
+    <t>In English: alisha, basanta, biwesh, jyoti, samir, sampana, shiva, siddhartha, sudip
+In Science: alisha, biwesh, jyoti, samir, sampana, shiva, siddhartha
+In Maths: biwesh, jyoti, samir, sampana, shiva, siddhartha
+In Social and Moral: alisha, biwesh, jamuna, jyoti, pari, samjhana, sanshila, siddhartha</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,8 +2027,47 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF00B050"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -288,8 +2104,62 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -405,11 +2275,52 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -443,9 +2354,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -455,6 +2363,58 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -541,7 +2501,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$A$2:$I$14" spid="_x0000_s1249"/>
+                  <a14:cameraTool cellRange="$A$2:$I$14" spid="_x0000_s1590"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -612,7 +2572,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$A$1:$K$19" spid="_x0000_s2185"/>
+                  <a14:cameraTool cellRange="$A$1:$K$19" spid="_x0000_s2526"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -628,6 +2588,77 @@
             <a:xfrm>
               <a:off x="14422581" y="0"/>
               <a:ext cx="13475623" cy="5158779"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>16234</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>205077</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>9</xdr:col>
+          <xdr:colOff>16234</xdr:colOff>
+          <xdr:row>28</xdr:row>
+          <xdr:rowOff>199215</xdr:rowOff>
+        </xdr:to>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="2" name="Picture 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82825E21-C29A-4A16-9566-CD6507258F5F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+              <a:extLst>
+                <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
+                  <a14:cameraTool cellRange="$A$2:$I$14" spid="_x0000_s3382"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+            <a:srcRect/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="16234" y="3628215"/>
+              <a:ext cx="10562492" cy="2965938"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -919,7 +2950,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1004,12 +3035,12 @@
         <v>15</v>
       </c>
       <c r="E3" s="6"/>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="25"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="54"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
@@ -1027,10 +3058,10 @@
       <c r="E4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="26"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="28"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="57"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
@@ -1048,10 +3079,10 @@
       <c r="E5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="26"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="28"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="56"/>
+      <c r="H5" s="56"/>
+      <c r="I5" s="57"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
@@ -1069,10 +3100,10 @@
       <c r="E6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="29"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="31"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="59"/>
+      <c r="H6" s="59"/>
+      <c r="I6" s="60"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
@@ -1286,8 +3317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C86ADD82-AA49-4A42-A6F1-3CD6CBA9B83D}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.21875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1338,20 +3369,20 @@
       <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="22" t="s">
         <v>15</v>
       </c>
       <c r="E2" s="13"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
       <c r="J2" s="14"/>
       <c r="K2" s="14"/>
     </row>
@@ -1359,22 +3390,22 @@
       <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
       <c r="J3" s="14"/>
       <c r="K3" s="14"/>
     </row>
@@ -1382,22 +3413,22 @@
       <c r="A4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="61"/>
       <c r="J4" s="14"/>
       <c r="K4" s="14"/>
     </row>
@@ -1405,22 +3436,22 @@
       <c r="A5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="61"/>
       <c r="J5" s="14"/>
       <c r="K5" s="14"/>
     </row>
@@ -1428,19 +3459,19 @@
       <c r="A6" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="24" t="s">
         <v>14</v>
       </c>
       <c r="G6" s="13"/>
@@ -1453,19 +3484,19 @@
       <c r="A7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="24" t="s">
         <v>15</v>
       </c>
       <c r="G7" s="13"/>
@@ -1478,19 +3509,19 @@
       <c r="A8" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="24" t="s">
         <v>13</v>
       </c>
       <c r="G8" s="13"/>
@@ -1503,19 +3534,19 @@
       <c r="A9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="24" t="s">
         <v>15</v>
       </c>
       <c r="G9" s="13"/>
@@ -1528,19 +3559,19 @@
       <c r="A10" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="24" t="s">
         <v>19</v>
       </c>
       <c r="G10" s="13"/>
@@ -1553,19 +3584,19 @@
       <c r="A11" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="24" t="s">
         <v>14</v>
       </c>
       <c r="G11" s="13"/>
@@ -1578,25 +3609,25 @@
       <c r="A12" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="G12" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="13" t="s">
+      <c r="H12" s="24" t="s">
         <v>21</v>
       </c>
       <c r="I12" s="13" t="s">
@@ -1609,25 +3640,25 @@
       <c r="A13" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="F13" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="15" t="s">
+      <c r="G13" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="15" t="s">
+      <c r="H13" s="26" t="s">
         <v>19</v>
       </c>
       <c r="I13" s="15" t="s">
@@ -1637,27 +3668,27 @@
       <c r="K13" s="14"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="33"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="34" t="s">
+      <c r="B14" s="62"/>
+      <c r="C14" s="62"/>
+      <c r="D14" s="63" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="34"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="63"/>
+      <c r="G14" s="63"/>
+      <c r="H14" s="63"/>
+      <c r="I14" s="63"/>
+      <c r="J14" s="63"/>
+      <c r="K14" s="63"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="21" t="s">
         <v>35</v>
       </c>
       <c r="C15" s="17" t="s">
@@ -1692,101 +3723,101 @@
       <c r="A16" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="21" t="s">
         <v>37</v>
       </c>
       <c r="C16" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="E16" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="F16" s="19" t="s">
+      <c r="F16" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="G16" s="19" t="s">
+      <c r="G16" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="H16" s="19" t="s">
+      <c r="H16" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="I16" s="19" t="s">
+      <c r="I16" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="J16" s="19" t="s">
+      <c r="J16" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="K16" s="19" t="s">
+      <c r="K16" s="25" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="8" customFormat="1" ht="54" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" s="8" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="D17" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="E17" s="21" t="s">
+      <c r="E17" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="F17" s="21" t="s">
+      <c r="F17" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="G17" s="21" t="s">
+      <c r="G17" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="H17" s="21" t="s">
+      <c r="H17" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="I17" s="21" t="s">
+      <c r="I17" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="J17" s="21" t="s">
+      <c r="J17" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="K17" s="21" t="s">
+      <c r="K17" s="20" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="35"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="35"/>
+      <c r="B18" s="64"/>
+      <c r="C18" s="64"/>
+      <c r="D18" s="64"/>
+      <c r="E18" s="64"/>
+      <c r="F18" s="64"/>
+      <c r="G18" s="64"/>
+      <c r="H18" s="64"/>
+      <c r="I18" s="64"/>
+      <c r="J18" s="64"/>
+      <c r="K18" s="64"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="35"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="35"/>
-      <c r="K19" s="35"/>
+      <c r="B19" s="64"/>
+      <c r="C19" s="64"/>
+      <c r="D19" s="64"/>
+      <c r="E19" s="64"/>
+      <c r="F19" s="64"/>
+      <c r="G19" s="64"/>
+      <c r="H19" s="64"/>
+      <c r="I19" s="64"/>
+      <c r="J19" s="64"/>
+      <c r="K19" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1801,4 +3832,2242 @@
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{565E6FEA-BE35-413C-A09C-8CD85F75B170}">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="47.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2">
+        <v>65038</v>
+      </c>
+      <c r="C2" s="2">
+        <v>65039</v>
+      </c>
+      <c r="D2" s="2">
+        <v>65040</v>
+      </c>
+      <c r="E2" s="2">
+        <v>65041</v>
+      </c>
+      <c r="F2" s="2">
+        <v>65042</v>
+      </c>
+      <c r="G2" s="2">
+        <v>65043</v>
+      </c>
+      <c r="H2" s="2">
+        <v>65044</v>
+      </c>
+      <c r="I2" s="2">
+        <v>65045</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="54"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="55"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="57"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="55"/>
+      <c r="G5" s="56"/>
+      <c r="H5" s="56"/>
+      <c r="I5" s="57"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="58"/>
+      <c r="G6" s="59"/>
+      <c r="H6" s="59"/>
+      <c r="I6" s="60"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" s="27" t="s">
+        <v>347</v>
+      </c>
+      <c r="J14" s="28" t="s">
+        <v>353</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F3:I6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC67C581-A697-447E-AF4F-2F9A0118EA18}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="49.5546875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="9" style="5"/>
+    <col min="3" max="3" width="92.21875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="9" style="5"/>
+    <col min="5" max="5" width="43.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="44" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="72" x14ac:dyDescent="0.35">
+      <c r="A2" s="48" t="s">
+        <v>354</v>
+      </c>
+      <c r="C2" s="48" t="s">
+        <v>356</v>
+      </c>
+      <c r="E2" s="44" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="36" x14ac:dyDescent="0.35">
+      <c r="A4" s="45" t="s">
+        <v>355</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>359</v>
+      </c>
+      <c r="E4" s="45" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="41" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="46" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="108" x14ac:dyDescent="0.35">
+      <c r="A6" s="43" t="s">
+        <v>344</v>
+      </c>
+      <c r="C6" s="47" t="s">
+        <v>360</v>
+      </c>
+      <c r="E6" s="47" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="42" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="90" x14ac:dyDescent="0.35">
+      <c r="A8" s="49" t="s">
+        <v>357</v>
+      </c>
+      <c r="C8" s="49" t="s">
+        <v>358</v>
+      </c>
+      <c r="E8" s="42" t="s">
+        <v>346</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A81E54D-8745-4ADD-9B3A-FA85F4902E2D}">
+  <dimension ref="A1:R44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="30.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="32.77734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="I1" s="36" t="s">
+        <v>210</v>
+      </c>
+      <c r="J1" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="K1" s="33" t="s">
+        <v>243</v>
+      </c>
+      <c r="L1" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="M1" s="37" t="s">
+        <v>273</v>
+      </c>
+      <c r="N1" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="O1" s="38" t="s">
+        <v>297</v>
+      </c>
+      <c r="P1" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q1" s="40" t="s">
+        <v>343</v>
+      </c>
+      <c r="R1" s="40" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" s="29"/>
+      <c r="C2" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>342</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>342</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="H2" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="I2" s="36" t="s">
+        <v>211</v>
+      </c>
+      <c r="J2" s="36"/>
+      <c r="K2" s="33" t="s">
+        <v>244</v>
+      </c>
+      <c r="L2" s="33"/>
+      <c r="M2" s="37" t="s">
+        <v>274</v>
+      </c>
+      <c r="N2" s="37"/>
+      <c r="O2" s="38" t="s">
+        <v>298</v>
+      </c>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="R2" s="40"/>
+    </row>
+    <row r="3" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A3" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>342</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="32"/>
+      <c r="G3" s="31" t="s">
+        <v>172</v>
+      </c>
+      <c r="H3" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="I3" s="36" t="s">
+        <v>212</v>
+      </c>
+      <c r="J3" s="36"/>
+      <c r="K3" s="33" t="s">
+        <v>245</v>
+      </c>
+      <c r="L3" s="33"/>
+      <c r="M3" s="37" t="s">
+        <v>275</v>
+      </c>
+      <c r="N3" s="37"/>
+      <c r="O3" s="38" t="s">
+        <v>299</v>
+      </c>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="40" t="s">
+        <v>321</v>
+      </c>
+      <c r="R3" s="40"/>
+    </row>
+    <row r="4" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A4" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>342</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>342</v>
+      </c>
+      <c r="G4" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="H4" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="I4" s="36" t="s">
+        <v>213</v>
+      </c>
+      <c r="J4" s="36"/>
+      <c r="K4" s="33" t="s">
+        <v>246</v>
+      </c>
+      <c r="L4" s="33"/>
+      <c r="M4" s="37" t="s">
+        <v>276</v>
+      </c>
+      <c r="N4" s="37"/>
+      <c r="O4" s="38" t="s">
+        <v>300</v>
+      </c>
+      <c r="P4" s="39"/>
+      <c r="Q4" s="40" t="s">
+        <v>322</v>
+      </c>
+      <c r="R4" s="40"/>
+    </row>
+    <row r="5" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A5" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>342</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>342</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>174</v>
+      </c>
+      <c r="H5" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="I5" s="36" t="s">
+        <v>214</v>
+      </c>
+      <c r="J5" s="36"/>
+      <c r="K5" s="33" t="s">
+        <v>247</v>
+      </c>
+      <c r="L5" s="33"/>
+      <c r="M5" s="37" t="s">
+        <v>277</v>
+      </c>
+      <c r="N5" s="37"/>
+      <c r="O5" s="38" t="s">
+        <v>301</v>
+      </c>
+      <c r="P5" s="39"/>
+      <c r="Q5" s="40" t="s">
+        <v>323</v>
+      </c>
+      <c r="R5" s="40"/>
+    </row>
+    <row r="6" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A6" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" s="29"/>
+      <c r="C6" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>342</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" s="32"/>
+      <c r="G6" s="31" t="s">
+        <v>175</v>
+      </c>
+      <c r="H6" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="I6" s="36" t="s">
+        <v>215</v>
+      </c>
+      <c r="J6" s="36"/>
+      <c r="K6" s="33" t="s">
+        <v>248</v>
+      </c>
+      <c r="L6" s="33"/>
+      <c r="M6" s="37" t="s">
+        <v>278</v>
+      </c>
+      <c r="N6" s="37"/>
+      <c r="O6" s="38" t="s">
+        <v>302</v>
+      </c>
+      <c r="P6" s="39"/>
+      <c r="Q6" s="40" t="s">
+        <v>324</v>
+      </c>
+      <c r="R6" s="40"/>
+    </row>
+    <row r="7" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A7" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>342</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="32"/>
+      <c r="G7" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="H7" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="I7" s="36" t="s">
+        <v>216</v>
+      </c>
+      <c r="J7" s="36"/>
+      <c r="K7" s="33" t="s">
+        <v>249</v>
+      </c>
+      <c r="L7" s="33"/>
+      <c r="M7" s="37" t="s">
+        <v>279</v>
+      </c>
+      <c r="N7" s="37"/>
+      <c r="O7" s="38" t="s">
+        <v>303</v>
+      </c>
+      <c r="P7" s="39"/>
+      <c r="Q7" s="40" t="s">
+        <v>325</v>
+      </c>
+      <c r="R7" s="40"/>
+    </row>
+    <row r="8" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A8" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" s="35"/>
+      <c r="E8" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" s="32"/>
+      <c r="G8" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="H8" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="I8" s="36" t="s">
+        <v>217</v>
+      </c>
+      <c r="J8" s="36"/>
+      <c r="K8" s="33" t="s">
+        <v>250</v>
+      </c>
+      <c r="L8" s="33"/>
+      <c r="M8" s="37" t="s">
+        <v>280</v>
+      </c>
+      <c r="N8" s="37"/>
+      <c r="O8" s="38" t="s">
+        <v>304</v>
+      </c>
+      <c r="P8" s="39"/>
+      <c r="Q8" s="40" t="s">
+        <v>326</v>
+      </c>
+      <c r="R8" s="40"/>
+    </row>
+    <row r="9" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A9" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9" s="29"/>
+      <c r="C9" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>342</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9" s="32"/>
+      <c r="G9" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="H9" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="I9" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="J9" s="36"/>
+      <c r="K9" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="L9" s="33"/>
+      <c r="M9" s="37" t="s">
+        <v>281</v>
+      </c>
+      <c r="N9" s="37"/>
+      <c r="O9" s="38" t="s">
+        <v>305</v>
+      </c>
+      <c r="P9" s="39"/>
+      <c r="Q9" s="40" t="s">
+        <v>327</v>
+      </c>
+      <c r="R9" s="40"/>
+    </row>
+    <row r="10" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A10" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="D10" s="35"/>
+      <c r="E10" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" s="32"/>
+      <c r="G10" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="H10" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="I10" s="36" t="s">
+        <v>219</v>
+      </c>
+      <c r="J10" s="36"/>
+      <c r="K10" s="33" t="s">
+        <v>252</v>
+      </c>
+      <c r="L10" s="33"/>
+      <c r="M10" s="37" t="s">
+        <v>282</v>
+      </c>
+      <c r="N10" s="37"/>
+      <c r="O10" s="38" t="s">
+        <v>306</v>
+      </c>
+      <c r="P10" s="39"/>
+      <c r="Q10" s="40" t="s">
+        <v>328</v>
+      </c>
+      <c r="R10" s="40"/>
+    </row>
+    <row r="11" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A11" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11" s="29"/>
+      <c r="C11" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11" s="35" t="s">
+        <v>342</v>
+      </c>
+      <c r="E11" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="F11" s="32"/>
+      <c r="G11" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="H11" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="I11" s="36" t="s">
+        <v>220</v>
+      </c>
+      <c r="J11" s="36"/>
+      <c r="K11" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="L11" s="33"/>
+      <c r="M11" s="37" t="s">
+        <v>283</v>
+      </c>
+      <c r="N11" s="37"/>
+      <c r="O11" s="38" t="s">
+        <v>307</v>
+      </c>
+      <c r="P11" s="39"/>
+      <c r="Q11" s="40" t="s">
+        <v>329</v>
+      </c>
+      <c r="R11" s="40"/>
+    </row>
+    <row r="12" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A12" s="29" t="s">
+        <v>140</v>
+      </c>
+      <c r="B12" s="29"/>
+      <c r="C12" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>342</v>
+      </c>
+      <c r="E12" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="F12" s="32" t="s">
+        <v>342</v>
+      </c>
+      <c r="G12" s="31" t="s">
+        <v>180</v>
+      </c>
+      <c r="H12" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="I12" s="36" t="s">
+        <v>221</v>
+      </c>
+      <c r="J12" s="36"/>
+      <c r="K12" s="33" t="s">
+        <v>254</v>
+      </c>
+      <c r="L12" s="33"/>
+      <c r="M12" s="37" t="s">
+        <v>284</v>
+      </c>
+      <c r="N12" s="37"/>
+      <c r="O12" s="38" t="s">
+        <v>308</v>
+      </c>
+      <c r="P12" s="39"/>
+      <c r="Q12" s="40" t="s">
+        <v>330</v>
+      </c>
+      <c r="R12" s="40"/>
+    </row>
+    <row r="13" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A13" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>342</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="F13" s="32" t="s">
+        <v>342</v>
+      </c>
+      <c r="G13" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="H13" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="I13" s="36" t="s">
+        <v>222</v>
+      </c>
+      <c r="J13" s="36"/>
+      <c r="K13" s="33" t="s">
+        <v>255</v>
+      </c>
+      <c r="L13" s="33"/>
+      <c r="M13" s="37" t="s">
+        <v>285</v>
+      </c>
+      <c r="N13" s="37"/>
+      <c r="O13" s="38" t="s">
+        <v>309</v>
+      </c>
+      <c r="P13" s="39"/>
+      <c r="Q13" s="40" t="s">
+        <v>331</v>
+      </c>
+      <c r="R13" s="40"/>
+    </row>
+    <row r="14" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A14" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="D14" s="35" t="s">
+        <v>342</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="F14" s="32"/>
+      <c r="G14" s="31" t="s">
+        <v>182</v>
+      </c>
+      <c r="H14" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="I14" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="J14" s="36"/>
+      <c r="K14" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="L14" s="33"/>
+      <c r="M14" s="37" t="s">
+        <v>286</v>
+      </c>
+      <c r="N14" s="37"/>
+      <c r="O14" s="38" t="s">
+        <v>310</v>
+      </c>
+      <c r="P14" s="39"/>
+      <c r="Q14" s="40" t="s">
+        <v>332</v>
+      </c>
+      <c r="R14" s="40"/>
+    </row>
+    <row r="15" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A15" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="B15" s="29"/>
+      <c r="C15" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>342</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="F15" s="32" t="s">
+        <v>342</v>
+      </c>
+      <c r="G15" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="H15" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="I15" s="36" t="s">
+        <v>224</v>
+      </c>
+      <c r="J15" s="36"/>
+      <c r="K15" s="33" t="s">
+        <v>257</v>
+      </c>
+      <c r="L15" s="33"/>
+      <c r="M15" s="37" t="s">
+        <v>287</v>
+      </c>
+      <c r="N15" s="37"/>
+      <c r="O15" s="38" t="s">
+        <v>311</v>
+      </c>
+      <c r="P15" s="39"/>
+      <c r="Q15" s="40" t="s">
+        <v>333</v>
+      </c>
+      <c r="R15" s="40"/>
+    </row>
+    <row r="16" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A16" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>342</v>
+      </c>
+      <c r="E16" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="F16" s="32" t="s">
+        <v>342</v>
+      </c>
+      <c r="G16" s="31" t="s">
+        <v>184</v>
+      </c>
+      <c r="H16" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="I16" s="36" t="s">
+        <v>225</v>
+      </c>
+      <c r="J16" s="36"/>
+      <c r="K16" s="33" t="s">
+        <v>258</v>
+      </c>
+      <c r="L16" s="33"/>
+      <c r="M16" s="37" t="s">
+        <v>288</v>
+      </c>
+      <c r="N16" s="37"/>
+      <c r="O16" s="38" t="s">
+        <v>312</v>
+      </c>
+      <c r="P16" s="39"/>
+      <c r="Q16" s="40" t="s">
+        <v>334</v>
+      </c>
+      <c r="R16" s="40"/>
+    </row>
+    <row r="17" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A17" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>119</v>
+      </c>
+      <c r="D17" s="35" t="s">
+        <v>342</v>
+      </c>
+      <c r="E17" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="F17" s="32" t="s">
+        <v>342</v>
+      </c>
+      <c r="G17" s="31" t="s">
+        <v>185</v>
+      </c>
+      <c r="H17" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="I17" s="36" t="s">
+        <v>226</v>
+      </c>
+      <c r="J17" s="36"/>
+      <c r="K17" s="33" t="s">
+        <v>259</v>
+      </c>
+      <c r="L17" s="33"/>
+      <c r="M17" s="37" t="s">
+        <v>289</v>
+      </c>
+      <c r="N17" s="37"/>
+      <c r="O17" s="38" t="s">
+        <v>313</v>
+      </c>
+      <c r="P17" s="39"/>
+      <c r="Q17" s="40" t="s">
+        <v>335</v>
+      </c>
+      <c r="R17" s="40"/>
+    </row>
+    <row r="18" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A18" s="29" t="s">
+        <v>146</v>
+      </c>
+      <c r="B18" s="29"/>
+      <c r="C18" s="34" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18" s="35" t="s">
+        <v>342</v>
+      </c>
+      <c r="E18" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="F18" s="32"/>
+      <c r="G18" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="H18" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="I18" s="36" t="s">
+        <v>227</v>
+      </c>
+      <c r="J18" s="36"/>
+      <c r="K18" s="33" t="s">
+        <v>260</v>
+      </c>
+      <c r="L18" s="33"/>
+      <c r="M18" s="37" t="s">
+        <v>290</v>
+      </c>
+      <c r="N18" s="37"/>
+      <c r="O18" s="38" t="s">
+        <v>314</v>
+      </c>
+      <c r="P18" s="39"/>
+      <c r="Q18" s="40" t="s">
+        <v>336</v>
+      </c>
+      <c r="R18" s="40"/>
+    </row>
+    <row r="19" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A19" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="D19" s="35" t="s">
+        <v>342</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="F19" s="32" t="s">
+        <v>342</v>
+      </c>
+      <c r="G19" s="31" t="s">
+        <v>187</v>
+      </c>
+      <c r="H19" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="I19" s="36" t="s">
+        <v>228</v>
+      </c>
+      <c r="J19" s="36"/>
+      <c r="K19" s="33" t="s">
+        <v>261</v>
+      </c>
+      <c r="L19" s="33"/>
+      <c r="M19" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="N19" s="37"/>
+      <c r="O19" s="38" t="s">
+        <v>315</v>
+      </c>
+      <c r="P19" s="39"/>
+      <c r="Q19" s="40" t="s">
+        <v>337</v>
+      </c>
+      <c r="R19" s="40"/>
+    </row>
+    <row r="20" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A20" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="B20" s="29"/>
+      <c r="C20" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="D20" s="35"/>
+      <c r="E20" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="F20" s="32"/>
+      <c r="G20" s="31" t="s">
+        <v>188</v>
+      </c>
+      <c r="H20" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="I20" s="36" t="s">
+        <v>229</v>
+      </c>
+      <c r="J20" s="36"/>
+      <c r="K20" s="33" t="s">
+        <v>262</v>
+      </c>
+      <c r="L20" s="33"/>
+      <c r="M20" s="37" t="s">
+        <v>292</v>
+      </c>
+      <c r="N20" s="37"/>
+      <c r="O20" s="38" t="s">
+        <v>316</v>
+      </c>
+      <c r="P20" s="39"/>
+      <c r="Q20" s="40" t="s">
+        <v>338</v>
+      </c>
+      <c r="R20" s="40"/>
+    </row>
+    <row r="21" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A21" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="D21" s="35"/>
+      <c r="E21" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="F21" s="32"/>
+      <c r="G21" s="31" t="s">
+        <v>189</v>
+      </c>
+      <c r="H21" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="I21" s="36" t="s">
+        <v>230</v>
+      </c>
+      <c r="J21" s="36"/>
+      <c r="K21" s="33" t="s">
+        <v>263</v>
+      </c>
+      <c r="L21" s="33"/>
+      <c r="M21" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="N21" s="37"/>
+      <c r="O21" s="38" t="s">
+        <v>317</v>
+      </c>
+      <c r="P21" s="39"/>
+      <c r="Q21" s="40" t="s">
+        <v>339</v>
+      </c>
+      <c r="R21" s="40"/>
+    </row>
+    <row r="22" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A22" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="B22" s="29"/>
+      <c r="C22" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="D22" s="35" t="s">
+        <v>342</v>
+      </c>
+      <c r="E22" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="F22" s="32" t="s">
+        <v>342</v>
+      </c>
+      <c r="G22" s="31" t="s">
+        <v>190</v>
+      </c>
+      <c r="H22" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="I22" s="36" t="s">
+        <v>231</v>
+      </c>
+      <c r="J22" s="36"/>
+      <c r="K22" s="33" t="s">
+        <v>264</v>
+      </c>
+      <c r="L22" s="33"/>
+      <c r="M22" s="37" t="s">
+        <v>294</v>
+      </c>
+      <c r="N22" s="37"/>
+      <c r="O22" s="38" t="s">
+        <v>318</v>
+      </c>
+      <c r="P22" s="39"/>
+      <c r="Q22" s="40" t="s">
+        <v>340</v>
+      </c>
+      <c r="R22" s="40"/>
+    </row>
+    <row r="23" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A23" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="D23" s="35" t="s">
+        <v>342</v>
+      </c>
+      <c r="E23" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="F23" s="32" t="s">
+        <v>342</v>
+      </c>
+      <c r="G23" s="31" t="s">
+        <v>191</v>
+      </c>
+      <c r="H23" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="I23" s="36" t="s">
+        <v>232</v>
+      </c>
+      <c r="J23" s="36"/>
+      <c r="K23" s="33" t="s">
+        <v>265</v>
+      </c>
+      <c r="L23" s="33"/>
+      <c r="M23" s="37" t="s">
+        <v>295</v>
+      </c>
+      <c r="N23" s="37"/>
+      <c r="O23" s="38" t="s">
+        <v>319</v>
+      </c>
+      <c r="P23" s="39"/>
+      <c r="Q23" s="40" t="s">
+        <v>341</v>
+      </c>
+      <c r="R23" s="40"/>
+    </row>
+    <row r="24" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A24" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="C24" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="D24" s="35" t="s">
+        <v>342</v>
+      </c>
+      <c r="E24" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="F24" s="32" t="s">
+        <v>342</v>
+      </c>
+      <c r="G24" s="31" t="s">
+        <v>192</v>
+      </c>
+      <c r="H24" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="I24" s="36" t="s">
+        <v>233</v>
+      </c>
+      <c r="J24" s="36"/>
+      <c r="K24" s="33" t="s">
+        <v>266</v>
+      </c>
+      <c r="L24" s="33"/>
+      <c r="M24" s="37" t="s">
+        <v>296</v>
+      </c>
+      <c r="N24" s="37"/>
+      <c r="O24" s="5"/>
+      <c r="P24">
+        <f>COUNTIF(P2:P23,"P")</f>
+        <v>0</v>
+      </c>
+      <c r="Q24" s="5"/>
+      <c r="R24">
+        <f>COUNTIF(R2:R23,"P")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A25" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="B25" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="C25" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="D25" s="35" t="s">
+        <v>342</v>
+      </c>
+      <c r="E25" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="F25" s="32" t="s">
+        <v>342</v>
+      </c>
+      <c r="G25" s="31" t="s">
+        <v>193</v>
+      </c>
+      <c r="H25" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="I25" s="36" t="s">
+        <v>234</v>
+      </c>
+      <c r="J25" s="36"/>
+      <c r="K25" s="33" t="s">
+        <v>267</v>
+      </c>
+      <c r="L25" s="33"/>
+      <c r="M25" s="5"/>
+      <c r="N25">
+        <f>COUNTIF(N2:N24,"P")</f>
+        <v>0</v>
+      </c>
+      <c r="O25" s="5"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="5"/>
+    </row>
+    <row r="26" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A26" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="C26" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="D26" s="35"/>
+      <c r="E26" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="F26" s="32" t="s">
+        <v>342</v>
+      </c>
+      <c r="G26" s="31" t="s">
+        <v>194</v>
+      </c>
+      <c r="H26" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="I26" s="36" t="s">
+        <v>235</v>
+      </c>
+      <c r="J26" s="36"/>
+      <c r="K26" s="33" t="s">
+        <v>268</v>
+      </c>
+      <c r="L26" s="33"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="5"/>
+      <c r="R26" s="5"/>
+    </row>
+    <row r="27" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A27" s="29" t="s">
+        <v>155</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5">
+        <f>COUNTIF(D2:D26,"P")</f>
+        <v>20</v>
+      </c>
+      <c r="E27" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="F27" s="32" t="s">
+        <v>342</v>
+      </c>
+      <c r="G27" s="31" t="s">
+        <v>195</v>
+      </c>
+      <c r="H27" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="I27" s="36" t="s">
+        <v>236</v>
+      </c>
+      <c r="J27" s="36"/>
+      <c r="K27" s="33" t="s">
+        <v>269</v>
+      </c>
+      <c r="L27" s="33"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
+    </row>
+    <row r="28" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A28" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="B28" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="F28" s="32" t="s">
+        <v>342</v>
+      </c>
+      <c r="G28" s="31" t="s">
+        <v>196</v>
+      </c>
+      <c r="H28" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="I28" s="36" t="s">
+        <v>237</v>
+      </c>
+      <c r="J28" s="36"/>
+      <c r="K28" s="33" t="s">
+        <v>270</v>
+      </c>
+      <c r="L28" s="33"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="5"/>
+    </row>
+    <row r="29" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A29" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="B29" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="F29" s="32" t="s">
+        <v>342</v>
+      </c>
+      <c r="G29" s="31" t="s">
+        <v>197</v>
+      </c>
+      <c r="H29" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="I29" s="36" t="s">
+        <v>238</v>
+      </c>
+      <c r="J29" s="36"/>
+      <c r="K29" s="33" t="s">
+        <v>271</v>
+      </c>
+      <c r="L29" s="33"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="5"/>
+    </row>
+    <row r="30" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A30" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="B30" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="F30" s="32" t="s">
+        <v>342</v>
+      </c>
+      <c r="G30" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="H30" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="I30" s="36" t="s">
+        <v>239</v>
+      </c>
+      <c r="J30" s="36"/>
+      <c r="K30" s="33" t="s">
+        <v>272</v>
+      </c>
+      <c r="L30" s="33"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="5"/>
+      <c r="R30" s="5"/>
+    </row>
+    <row r="31" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A31" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="B31" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="F31" s="32" t="s">
+        <v>342</v>
+      </c>
+      <c r="G31" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="H31" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="I31" s="36" t="s">
+        <v>240</v>
+      </c>
+      <c r="J31" s="36"/>
+      <c r="K31" s="5"/>
+      <c r="L31">
+        <f>COUNTIF(L2:L30,"P")</f>
+        <v>0</v>
+      </c>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
+      <c r="P31" s="5"/>
+      <c r="Q31" s="5"/>
+      <c r="R31" s="5"/>
+    </row>
+    <row r="32" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A32" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="B32" s="29"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="F32" s="32" t="s">
+        <v>342</v>
+      </c>
+      <c r="G32" s="31" t="s">
+        <v>200</v>
+      </c>
+      <c r="H32" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="I32" s="36" t="s">
+        <v>241</v>
+      </c>
+      <c r="J32" s="36"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="5"/>
+      <c r="P32" s="5"/>
+      <c r="Q32" s="5"/>
+      <c r="R32" s="5"/>
+    </row>
+    <row r="33" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A33" s="29" t="s">
+        <v>161</v>
+      </c>
+      <c r="B33" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="F33" s="32" t="s">
+        <v>342</v>
+      </c>
+      <c r="G33" s="31" t="s">
+        <v>201</v>
+      </c>
+      <c r="H33" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="I33" s="36" t="s">
+        <v>242</v>
+      </c>
+      <c r="J33" s="36"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="5"/>
+      <c r="P33" s="5"/>
+      <c r="Q33" s="5"/>
+      <c r="R33" s="5"/>
+    </row>
+    <row r="34" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A34" s="29" t="s">
+        <v>162</v>
+      </c>
+      <c r="B34" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="F34" s="32" t="s">
+        <v>342</v>
+      </c>
+      <c r="G34" s="31" t="s">
+        <v>168</v>
+      </c>
+      <c r="H34" s="31"/>
+      <c r="I34" s="5"/>
+      <c r="J34">
+        <f>COUNTIF(J2:J33,"P")</f>
+        <v>0</v>
+      </c>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="5"/>
+      <c r="P34" s="5"/>
+      <c r="Q34" s="5"/>
+      <c r="R34" s="5"/>
+    </row>
+    <row r="35" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A35" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="B35" s="29"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="F35" s="32"/>
+      <c r="G35" s="31" t="s">
+        <v>202</v>
+      </c>
+      <c r="H35" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="5"/>
+      <c r="O35" s="5"/>
+      <c r="P35" s="5"/>
+      <c r="Q35" s="5"/>
+      <c r="R35" s="5"/>
+    </row>
+    <row r="36" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A36" s="29" t="s">
+        <v>164</v>
+      </c>
+      <c r="B36" s="29"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F36" s="32" t="s">
+        <v>342</v>
+      </c>
+      <c r="G36" s="31" t="s">
+        <v>203</v>
+      </c>
+      <c r="H36" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="5"/>
+      <c r="O36" s="5"/>
+      <c r="P36" s="5"/>
+      <c r="Q36" s="5"/>
+      <c r="R36" s="5"/>
+    </row>
+    <row r="37" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A37" s="29" t="s">
+        <v>165</v>
+      </c>
+      <c r="B37" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="F37" s="32" t="s">
+        <v>342</v>
+      </c>
+      <c r="G37" s="31" t="s">
+        <v>204</v>
+      </c>
+      <c r="H37" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="5"/>
+      <c r="N37" s="5"/>
+      <c r="O37" s="5"/>
+      <c r="P37" s="5"/>
+      <c r="Q37" s="5"/>
+      <c r="R37" s="5"/>
+    </row>
+    <row r="38" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A38" s="29" t="s">
+        <v>166</v>
+      </c>
+      <c r="B38" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38">
+        <f>COUNTIF(F2:F37,"P")</f>
+        <v>24</v>
+      </c>
+      <c r="G38" s="31" t="s">
+        <v>205</v>
+      </c>
+      <c r="H38" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="5"/>
+      <c r="N38" s="5"/>
+      <c r="O38" s="5"/>
+      <c r="P38" s="5"/>
+      <c r="Q38" s="5"/>
+      <c r="R38" s="5"/>
+    </row>
+    <row r="39" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A39" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="B39" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="31" t="s">
+        <v>206</v>
+      </c>
+      <c r="H39" s="31"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5"/>
+      <c r="M39" s="5"/>
+      <c r="N39" s="5"/>
+      <c r="O39" s="5"/>
+      <c r="P39" s="5"/>
+      <c r="Q39" s="5"/>
+      <c r="R39" s="5"/>
+    </row>
+    <row r="40" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A40" s="29" t="s">
+        <v>168</v>
+      </c>
+      <c r="B40" s="29"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="31" t="s">
+        <v>207</v>
+      </c>
+      <c r="H40" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="5"/>
+      <c r="M40" s="5"/>
+      <c r="N40" s="5"/>
+      <c r="O40" s="5"/>
+      <c r="P40" s="5"/>
+      <c r="Q40" s="5"/>
+      <c r="R40" s="5"/>
+    </row>
+    <row r="41" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A41" s="29" t="s">
+        <v>169</v>
+      </c>
+      <c r="B41" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="H41" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5"/>
+      <c r="M41" s="5"/>
+      <c r="N41" s="5"/>
+      <c r="O41" s="5"/>
+      <c r="P41" s="5"/>
+      <c r="Q41" s="5"/>
+      <c r="R41" s="5"/>
+    </row>
+    <row r="42" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A42" s="29" t="s">
+        <v>170</v>
+      </c>
+      <c r="B42" s="29"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="H42" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="5"/>
+      <c r="L42" s="5"/>
+      <c r="M42" s="5"/>
+      <c r="N42" s="5"/>
+      <c r="O42" s="5"/>
+      <c r="P42" s="5"/>
+      <c r="Q42" s="5"/>
+      <c r="R42" s="5"/>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B43">
+        <f>COUNTIF(B2:B42,"P")</f>
+        <v>27</v>
+      </c>
+      <c r="H43">
+        <f>COUNTIF(H2:H42,"P")</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B44">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>